<commit_message>
agrega log trick a extension y materialize
</commit_message>
<xml_diff>
--- a/entrenamiento/corpus.xlsx
+++ b/entrenamiento/corpus.xlsx
@@ -1,217 +1,218 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgasca\Desktop\cesar\TT2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="95">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>etiqueta</t>
-  </si>
-  <si>
-    <t>Ha ganado (500,000.00 dólares) de la Lotería Nacional del Reino Unido, responda para reclamar su precio.</t>
-  </si>
-  <si>
-    <t>phishing</t>
-  </si>
-  <si>
-    <t>CÁMARAS DE JOHN ALBERT_x000D_
-DIRECCIÓN: MORELEY HOUSE, 26/30_x000D_
-VIABULT HOLLBORN_x000D_
-LONDRES EC 1 A2BP, Reino Unido_x000D_
-TEL: + (44) -7520-636-234_x000D_
- _x000D_
-_x000D_
-_x000D_
-NOTIFICACIÓN DE LEGADO_x000D_
- _x000D_
-Soy el abogado John Albert, en nombre de los Fideicomisarios y el Ejecutor de la herencia del difunto Sr. Harley Graham Wade, se me asignó contactarlo y notificarlo ya que mi carta anterior fue devuelta sin entregar. El Sr. Harley Graham Wade dejó la suma de tres millones quinientas mil libras (3,500,000.00 GBP) para usted en un número de cuenta bancaria: 30207712320 con CREDIT SUISSE BANK aquí en Londres, Reino Unido._x000D_
-_x000D_
-En el codicilo y último testamento de su VOLUNTAD bajo mi custodia. Hasta su muerte, fue una gran filantropía que le valió numerosos premios durante su vida. El fallecido Sr. Harley Graham Wade murió el 13 de diciembre de 2012 a la edad de 75 años, y sus fondos ahora están listos para la ejecución. Según él, este dinero es para apoyar actividades humanitarias y ayudar a los pobres, los necesitados y los indigentes de nuestra sociedad a su manera._x000D_
-_x000D_
-Por favor, trate de contactarme lo antes posible si me encuentro con usted esta vez, ya que tengo esperanzas, para permitirme concluir mi trabajo. Al responder a este correo electrónico, deberá actualizar el siguiente formulario para que pueda contactarlo y también enviarle el "FORMULARIO DE SOLICITUD DE CERTIFICADO DE DEBIDA DILIGENCIA" que deberá completar y enviar a la Cámara y al Banco de Depósito de Seguridad para reclamos correctos._x000D_
- _x000D_
-1. Nombre completo: _____________________x000D_
-2. Dirección: _______________________x000D_
-3. Ocupación: ____________________x000D_
-4. País de residencia: __________x000D_
-5. Tel: ___________________________x000D_
-6. Edad: ___________________________x000D_
-7. Nacionalidad: ___________________x000D_
- _x000D_
-Esta es mi dirección de contacto de correo electrónico personal:JohnAlbertChambers@legislator.com_x000D_
-Contácteme tan pronto como lea este correo electrónico para que podamos continuar con el envío y la obtención de la documentación legal que respalde la recepción de estos fondos. Espero tener noticias tuyas en poco tiempo._x000D_
-_x000D_
-Barr John Albert {Esq.}_x000D_
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="107">
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etiqueta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ha ganado (500,000.00 dólares) de la Lotería Nacional del Reino Unido, responda para reclamar su precio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CÁMARAS DE JOHN ALBERT_x005F_x000D_
+DIRECCIÓN: MORELEY HOUSE, 26/30_x005F_x000D_
+VIABULT HOLLBORN_x005F_x000D_
+LONDRES EC 1 A2BP, Reino Unido_x005F_x000D_
+TEL: + (44) -7520-636-234_x005F_x000D_
+ _x005F_x000D_
+_x005F_x000D_
+_x005F_x000D_
+NOTIFICACIÓN DE LEGADO_x005F_x000D_
+ _x005F_x000D_
+Soy el abogado John Albert, en nombre de los Fideicomisarios y el Ejecutor de la herencia del difunto Sr. Harley Graham Wade, se me asignó contactarlo y notificarlo ya que mi carta anterior fue devuelta sin entregar. El Sr. Harley Graham Wade dejó la suma de tres millones quinientas mil libras (3,500,000.00 GBP) para usted en un número de cuenta bancaria: 30207712320 con CREDIT SUISSE BANK aquí en Londres, Reino Unido._x005F_x000D_
+_x005F_x000D_
+En el codicilo y último testamento de su VOLUNTAD bajo mi custodia. Hasta su muerte, fue una gran filantropía que le valió numerosos premios durante su vida. El fallecido Sr. Harley Graham Wade murió el 13 de diciembre de 2012 a la edad de 75 años, y sus fondos ahora están listos para la ejecución. Según él, este dinero es para apoyar actividades humanitarias y ayudar a los pobres, los necesitados y los indigentes de nuestra sociedad a su manera._x005F_x000D_
+_x005F_x000D_
+Por favor, trate de contactarme lo antes posible si me encuentro con usted esta vez, ya que tengo esperanzas, para permitirme concluir mi trabajo. Al responder a este correo electrónico, deberá actualizar el siguiente formulario para que pueda contactarlo y también enviarle el "FORMULARIO DE SOLICITUD DE CERTIFICADO DE DEBIDA DILIGENCIA" que deberá completar y enviar a la Cámara y al Banco de Depósito de Seguridad para reclamos correctos._x005F_x000D_
+ _x005F_x000D_
+1. Nombre completo: _____________________x005F_x000D_
+2. Dirección: _______________________x005F_x000D_
+3. Ocupación: ____________________x005F_x000D_
+4. País de residencia: __________x005F_x000D_
+5. Tel: ___________________________x005F_x000D_
+6. Edad: ___________________________x005F_x000D_
+7. Nacionalidad: ___________________x005F_x000D_
+ _x005F_x000D_
+Esta es mi dirección de contacto de correo electrónico personal:JohnAlbertChambers@legislator.com_x005F_x000D_
+Contácteme tan pronto como lea este correo electrónico para que podamos continuar con el envío y la obtención de la documentación legal que respalde la recepción de estos fondos. Espero tener noticias tuyas en poco tiempo._x005F_x000D_
+_x005F_x000D_
+Barr John Albert {Esq.}_x005F_x000D_
 Abogado a cargo.</t>
   </si>
   <si>
-    <t>Estimado usuario de cuenta de correo electrónico:_x000D_
-_x000D_
-         Debido a tantos correos basura, actualmente estamos_x000D_
-actualizando nuestra base de datos para brindarle un mejor servicio._x000D_
-_x000D_
-Para continuar usando su cuenta, debe responder a este correo_x000D_
-electrónico proporcionando la siguiente información a continuación:_x000D_
-_x000D_
-Nombres completos: _x000D_
-Email: _x000D_
-Nombre de usuario: _x000D_
-Contraseña: _x000D_
-Confirmar contraseña: _x000D_
-Tel: _x000D_
-_x000D_
-Nota: Si no responde a este mensaje, su cuenta se desactivará desde_x000D_
-nuestra base de datos y ya no recibirá ni enviará correos electrónicos._x000D_
-_x000D_
-Nos disculpamos por cualquier inconveniente que esto pueda causarle._x000D_
-_x000D_
-Saludos,_x000D_
-_x000D_
+    <t xml:space="preserve">Estimado usuario de cuenta de correo electrónico:_x005F_x000D_
+_x005F_x000D_
+         Debido a tantos correos basura, actualmente estamos_x005F_x000D_
+actualizando nuestra base de datos para brindarle un mejor servicio._x005F_x000D_
+_x005F_x000D_
+Para continuar usando su cuenta, debe responder a este correo_x005F_x000D_
+electrónico proporcionando la siguiente información a continuación:_x005F_x000D_
+_x005F_x000D_
+Nombres completos: _x005F_x000D_
+Email: _x005F_x000D_
+Nombre de usuario: _x005F_x000D_
+Contraseña: _x005F_x000D_
+Confirmar contraseña: _x005F_x000D_
+Tel: _x005F_x000D_
+_x005F_x000D_
+Nota: Si no responde a este mensaje, su cuenta se desactivará desde_x005F_x000D_
+nuestra base de datos y ya no recibirá ni enviará correos electrónicos._x005F_x000D_
+_x005F_x000D_
+Nos disculpamos por cualquier inconveniente que esto pueda causarle._x005F_x000D_
+_x005F_x000D_
+Saludos,_x005F_x000D_
+_x005F_x000D_
 Administrador Sistema.</t>
   </si>
   <si>
-    <t>Como parte de nuestra decisión de mejorar nuestros servicios contra cualquier tratamiento de virus, debe actualizar su interfaz de correo electrónico dentro de las próximas 24 horas para permitirnos eliminar el virus HKN de su correo electrónico. Completa tu proceso._x000D_
-Email :_x000D_
-Nombre de usuario_x000D_
-Contraseña:_x000D_
-Vuelva a escribir la contraseña_x000D_
+    <t xml:space="preserve">Como parte de nuestra decisión de mejorar nuestros servicios contra cualquier tratamiento de virus, debe actualizar su interfaz de correo electrónico dentro de las próximas 24 horas para permitirnos eliminar el virus HKN de su correo electrónico. Completa tu proceso._x005F_x000D_
+Email :_x005F_x000D_
+Nombre de usuario_x005F_x000D_
+Contraseña:_x005F_x000D_
+Vuelva a escribir la contraseña_x005F_x000D_
 Advertencia El incumplimiento determinará su cuenta de correo electrónico.</t>
   </si>
   <si>
-    <t>Como parte de nuestra decisión de mejorar nuestros servicios de correo web, debe actualizar para una nueva interfaz de correo web para las próximas 4 horas. HAGA CLIC AQUÍ y complete la información correctamente. Advertencia: si no se actualiza, su cuenta de correo web se desactivará y suspenderá con 4 horas</t>
-  </si>
-  <si>
-    <t>ID de Apple bloqueado_x000D_
-Su ID de Apple ha sido bloqueada por razones de seguridad. 19 de enero, 2020 PST, para desbloquearlo, debes verificar tu identidad._x000D_
-_x000D_
-no puede acceder a su cuenta ni a ningún servicio de Apple antes de completar la verificación, y debe completar la verificación antes de las 12 horas o su cuenta se bloqueará permanentemente._x000D_
-_x000D_
+    <t xml:space="preserve">Como parte de nuestra decisión de mejorar nuestros servicios de correo web, debe actualizar para una nueva interfaz de correo web para las próximas 4 horas. HAGA CLIC AQUÍ y complete la información correctamente. Advertencia: si no se actualiza, su cuenta de correo web se desactivará y suspenderá con 4 horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID de Apple bloqueado_x005F_x000D_
+Su ID de Apple ha sido bloqueada por razones de seguridad. 19 de enero, 2020 PST, para desbloquearlo, debes verificar tu identidad._x005F_x000D_
+_x005F_x000D_
+no puede acceder a su cuenta ni a ningún servicio de Apple antes de completar la verificación, y debe completar la verificación antes de las 12 horas o su cuenta se bloqueará permanentemente._x005F_x000D_
+_x005F_x000D_
 Desbloquear cuenta.</t>
   </si>
   <si>
-    <t>Pago automático._x000D_
-Hola cliente_x000D_
-Su pago automático no puede procesarse._x000D_
-Su período de suscripción finalizará el viernes 24 de enero de 2020._x000D_
-Haga clic aquí para actualizar su método de pago_x000D_
-actualice su método de pago para continuar con la función de Netflix._x000D_
+    <t xml:space="preserve">Pago automático._x005F_x000D_
+Hola cliente_x005F_x000D_
+Su pago automático no puede procesarse._x005F_x000D_
+Su período de suscripción finalizará el viernes 24 de enero de 2020._x005F_x000D_
+Haga clic aquí para actualizar su método de pago_x005F_x000D_
+actualice su método de pago para continuar con la función de Netflix._x005F_x000D_
 El equipo de Netflix</t>
   </si>
   <si>
-    <t>shandella_1997 ¡SE NECESITA confirmación!_x000D_
-¡¡DARSE PRISA!! ¡OFERTA POR TIEMPO LIMITADO!_x000D_
-Parece que hay algo mal con su correo electrónico porque nosotros_x000D_
-he tratado de contactarte varias veces la semana pasada._x000D_
-Usted es elegido en nuestro sorteo anual para el consumidor para obtener un premio gratis como agradecimiento por ser actual o_x000D_
-Cliente fiel anterior._x000D_
-_x000D_
-Para calificar para esta oferta especial, simplemente complete nuestro marketing de 30 segundos_x000D_
+    <t xml:space="preserve">shandella_1997 ¡SE NECESITA confirmación!_x005F_x000D_
+¡¡DARSE PRISA!! ¡OFERTA POR TIEMPO LIMITADO!_x005F_x000D_
+Parece que hay algo mal con su correo electrónico porque nosotros_x005F_x000D_
+he tratado de contactarte varias veces la semana pasada._x005F_x000D_
+Usted es elegido en nuestro sorteo anual para el consumidor para obtener un premio gratis como agradecimiento por ser actual o_x005F_x000D_
+Cliente fiel anterior._x005F_x000D_
+_x005F_x000D_
+Para calificar para esta oferta especial, simplemente complete nuestro marketing de 30 segundos_x005F_x000D_
 encuesta sobre sus experiencias de compra</t>
   </si>
   <si>
-    <t>Asunto : Su tarjeta será suspendida_x000D_
-_x000D_
-Remitente : Servicio al cliente._x000D_
-Estimado Cliente ,_x000D_
-Estamos teniendo problemas para verificar la información de su tarjeta de crédito._x000D_
-Lo invitamos a corregir este problema haciendo clic en el enlace de abajo y siguiendo las instrucciones :_x000D_
+    <t xml:space="preserve">Asunto : Su tarjeta será suspendida_x005F_x000D_
+_x005F_x000D_
+Remitente : Servicio al cliente._x005F_x000D_
+Estimado Cliente ,_x005F_x000D_
+Estamos teniendo problemas para verificar la información de su tarjeta de crédito._x005F_x000D_
+Lo invitamos a corregir este problema haciendo clic en el enlace de abajo y siguiendo las instrucciones :_x005F_x000D_
 Haga clic aqui,y iniciar sesion en su cuenta</t>
   </si>
   <si>
-    <t>Su dirección de correo electrónico ha sido seleccionada como uno de nuestros afortunados ganadores para recibir una donación en efectivo de $ 850000 USD. Para más detalles, escríbanos</t>
-  </si>
-  <si>
-    <t>PayPal viernes, 17 de enero de 2020, 21:43:12 PM PDT Número de recibo: SE09157472768465_x000D_
-_x000D_
-Hola,_x000D_
-Ha enviado un pago de $ 134.90 USD a Oracle cloud, inc._x000D_
-Tenga en cuenta que esta transacción puede tardar unos minutos en aparecer en la descripción general de su cuenta._x000D_
-Ver los detalles de esta transacción en línea._x000D_
+    <t xml:space="preserve">Su dirección de correo electrónico ha sido seleccionada como uno de nuestros afortunados ganadores para recibir una donación en efectivo de $ 850000 USD. Para más detalles, escríbanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PayPal viernes, 17 de enero de 2020, 21:43:12 PM PDT Número de recibo: SE09157472768465_x005F_x000D_
+_x005F_x000D_
+Hola,_x005F_x000D_
+Ha enviado un pago de $ 134.90 USD a Oracle cloud, inc._x005F_x000D_
+Tenga en cuenta que esta transacción puede tardar unos minutos en aparecer en la descripción general de su cuenta._x005F_x000D_
+Ver los detalles de esta transacción en línea._x005F_x000D_
 Si no fue usted quien realizó esta transacción, puede disputar la transacción haciendo clic en resolver ahora</t>
   </si>
   <si>
-    <t xml:space="preserve">Querido_x000D_
-_x000D_
-Su factura NET acaba de llegar y para ver todos los detalles simplemente abra el documento adjunto a este correo electrónico._x000D_
-_x000D_
+    <t xml:space="preserve">Querido_x005F_x000D_
+_x005F_x000D_
+Su factura NET acaba de llegar y para ver todos los detalles simplemente abra el documento adjunto a este correo electrónico._x005F_x000D_
+_x005F_x000D_
 A continuación se muestra un resumen con la información principal. Y tenga la seguridad de que su pago de débito automático ya está programado. </t>
   </si>
   <si>
-    <t>Esta es mi merecida oportunidad para finalmente conocer a alguien para pasar muchas horas y días juntos._x000D_
-http://www.bbatsonjohn60.xyz_x000D_
- _x000D_
+    <t xml:space="preserve">Esta es mi merecida oportunidad para finalmente conocer a alguien para pasar muchas horas y días juntos._x005F_x000D_
+http://www.bbatsonjohn60.xyz_x005F_x000D_
+ _x005F_x000D_
 Paola</t>
   </si>
   <si>
-    <t>Estimado cliente_x000D_
-_x000D_
-Su cuenta de PayPal se utilizó para iniciar sesión en el nuevo dispositivo y realizar un pago a través de Google Play Store_x000D_
-_x000D_
-Este es el detalle de tu actividad._x000D_
-Artículo: apalancamiento en la muerte_x000D_
-Dispositivo: Linux, Android-Samsung S9 Plus_x000D_
-Fecha: jueves 13 de septiembre de 2018_x000D_
-_x000D_
-Cantidad total del pedido $ 17.99_x000D_
-Ubicación: Alburque Nuevo México, Estados Unidos_x000D_
-Dirección IP: 112.4.27.105_x000D_
-_x000D_
+    <t xml:space="preserve">Estimado cliente_x005F_x000D_
+_x005F_x000D_
+Su cuenta de PayPal se utilizó para iniciar sesión en el nuevo dispositivo y realizar un pago a través de Google Play Store_x005F_x000D_
+_x005F_x000D_
+Este es el detalle de tu actividad._x005F_x000D_
+Artículo: apalancamiento en la muerte_x005F_x000D_
+Dispositivo: Linux, Android-Samsung S9 Plus_x005F_x000D_
+Fecha: jueves 13 de septiembre de 2018_x005F_x000D_
+_x005F_x000D_
+Cantidad total del pedido $ 17.99_x005F_x000D_
+Ubicación: Alburque Nuevo México, Estados Unidos_x005F_x000D_
+Dirección IP: 112.4.27.105_x005F_x000D_
+_x005F_x000D_
 Si no realizó esta compra, informe este problema y cancele el pago en:</t>
   </si>
   <si>
-    <t>Estimado, cliente,_x000D_
-Estamos teniendo problemas para verificar la información de su tarjeta de crédito._x000D_
-Lo invitamos a corregir este problema haciendo click en el enlace de abajo y siguiendo las siguientes instruccions:_x000D_
+    <t xml:space="preserve">Estimado, cliente,_x005F_x000D_
+Estamos teniendo problemas para verificar la información de su tarjeta de crédito._x005F_x000D_
+Lo invitamos a corregir este problema haciendo click en el enlace de abajo y siguiendo las siguientes instruccions:_x005F_x000D_
 Haga clic aqui y iniciar sesión en su cuenta.</t>
   </si>
   <si>
-    <t>¿Estás en linea?</t>
-  </si>
-  <si>
-    <t>Estimado empleado, personal._x000D_
-_x000D_
-Estamos migrando toda la cuenta de correo electrónico del personal al correo web de la oficina Outlook 2020 del personal y, como tal, todo el personal y los empleados activos deben verificar e iniciar sesión para que esta actualización y migración surtan efecto ahora._x000D_
-Esto se hace para mejorar la seguridad y la eficiencia debido a los recientes correos no deseados recibidos._x000D_
-_x000D_
-Por favor, todo el personal y los empleados Haga clic aquí Cambiar a Outlook Webmail 2020 para el personal_x000D_
-_x000D_
-Tenga en cuenta que este cambio en Outlook es para todos los usuarios de correo electrónico en este servicio y, si no lo hace,_x000D_
-comenzaremos a desactivar y eliminar cuentas de correo electrónico no verificadas e inactivas sin más demora en las próximas 24 horas._x000D_
-POR FAVOR HAGA LAS ASESORACIONES ANTERIORES._x000D_
-_x000D_
-Saludos,_x000D_
-Administrador de correo electrónico externo,_x000D_
-Servicio de Outlook para personal y servicio de internet_x000D_
+    <t xml:space="preserve">¿Estás en linea?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimado empleado, personal._x005F_x000D_
+_x005F_x000D_
+Estamos migrando toda la cuenta de correo electrónico del personal al correo web de la oficina Outlook 2020 del personal y, como tal, todo el personal y los empleados activos deben verificar e iniciar sesión para que esta actualización y migración surtan efecto ahora._x005F_x000D_
+Esto se hace para mejorar la seguridad y la eficiencia debido a los recientes correos no deseados recibidos._x005F_x000D_
+_x005F_x000D_
+Por favor, todo el personal y los empleados Haga clic aquí Cambiar a Outlook Webmail 2020 para el personal_x005F_x000D_
+_x005F_x000D_
+Tenga en cuenta que este cambio en Outlook es para todos los usuarios de correo electrónico en este servicio y, si no lo hace,_x005F_x000D_
+comenzaremos a desactivar y eliminar cuentas de correo electrónico no verificadas e inactivas sin más demora en las próximas 24 horas._x005F_x000D_
+POR FAVOR HAGA LAS ASESORACIONES ANTERIORES._x005F_x000D_
+_x005F_x000D_
+Saludos,_x005F_x000D_
+Administrador de correo electrónico externo,_x005F_x000D_
+Servicio de Outlook para personal y servicio de internet_x005F_x000D_
 Copyright2020.</t>
   </si>
   <si>
-    <t>Estimado Cliente:_x000D_
-_x000D_
-Le informamos que su cuenta fue bloqueada, debido a que no a actualizado o activado sus alertas bbva._x000D_
-_x000D_
+    <t xml:space="preserve">Estimado Cliente:_x005F_x000D_
+_x005F_x000D_
+Le informamos que su cuenta fue bloqueada, debido a que no a actualizado o activado sus alertas bbva._x005F_x000D_
+_x005F_x000D_
 Para poder desbloquear imediatamente su tarjeta y poder seguir disfrutando los servicios de bbva.mx y bbva.movil es necesario ingresar al portal de bbva y hacer el proceso de activación o actualización de Alertas BBVA</t>
   </si>
   <si>
-    <t>VEHÍCULO MATRÍCULA: 9250CNP
+    <t xml:space="preserve">VEHÍCULO MATRÍCULA: 9250CNP
 FECHA LIMITE DE INSPECCION: 23/10/2011
 Estimado/a  Sr./Sra.:
 De acuerdo con los datos obtenidos en nuestro registro de inspeccións, a este vehículo le correspónde pasar a la PRÓXIMA INSPECCIÓN TECNICA no mas tarde de la fecha señalada , salvo que ya lo haya hecho.
@@ -646,7 +647,7 @@
 The equipo de CiteAlert
 ---------------------------------------------------------------------------
 Su articulo:
-Comportamiento del polen Platanis hispanica, un aeroalergeno importante dprimavera en la Espaa del noroeste</t>
+Comportamiento del polen Platanis hispanica, un aeroalergeno importante de primavera en la Espaa del noroeste</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1039,7 +1040,7 @@
 </t>
   </si>
   <si>
-    <t>Chicos, adjunto encontrarán un corte final en el presupuesto de gastos de ENA 2001.
+    <t xml:space="preserve">Chicos, adjunto encontrarán un corte final en el presupuesto de gastos de ENA 2001.
 Revisen y hagan los ajustes a su plan existente que sean
 apropiados para alcanzar el objetivo neto de ENA. Para permanecer plano año tras año, yo
 divido la varianza positiva restante por igual entre los grupos. Como lo hemos
@@ -1056,10 +1057,10 @@
 Delainey</t>
   </si>
   <si>
-    <t>ham</t>
-  </si>
-  <si>
-    <t>Todavía necesito información sobre el Plan de Mercados Globales. (Ver
+    <t xml:space="preserve">ham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todavía necesito información sobre el Plan de Mercados Globales. (Ver
 Correo electrónico previo)
   Si está en uno de los siguientes grupos, ¿podría responder con
 su desglose lo antes posible:
@@ -1073,7 +1074,7 @@
 3-5843</t>
   </si>
   <si>
-    <t>Se adjunta un archivo que contiene todos los centros de costos que se asignan a Global
+    <t xml:space="preserve">Se adjunta un archivo que contiene todos los centros de costos que se asignan a Global
 Mercados en el año 2001. ¿Podría darme un desglose de cada
 equipo afectado por los mercados globales. Por favor explique todos los porcentajes listados en
 columna "A", al dividirse en columnas B - J. No dude en llamar
@@ -1084,7 +1085,7 @@
 3-5843</t>
   </si>
   <si>
-    <t>Sarah
+    <t xml:space="preserve">Sarah
 A continuación se muestra nuestra explicación de alto nivel de las operaciones de energía (incluida la EOL)
 aumento en el plan de 2001 sobre el pronóstico de 2000 de $ 5,1 millones. Si tienes alguna
 pregunta, por favor hágamelo saber.
@@ -1098,13 +1099,13 @@
 Brian</t>
   </si>
   <si>
-    <t>Sally: comprobaré el significado de este correo electrónico y te responderé. yo
+    <t xml:space="preserve">Sally: comprobaré el significado de este correo electrónico y te responderé. yo
 pude dejarle un mensaje de correo de voz o darle la información a Patti.
 Lisa
 Enron North America Corp.</t>
   </si>
   <si>
-    <t>Tenga en cuenta que los ingresos y las plantillas de plantilla se deben a Consolidaciones
+    <t xml:space="preserve">Tenga en cuenta que los ingresos y las plantillas de plantilla se deben a Consolidaciones
 el lunes 2 de octubre. Se adjunta la última línea de tiempo. Por favor envíe su
 plantillas para Trey Hardy para entonces. Varias pautas o asignación
 no se le han enviado cálculos (por ejemplo, TI) porque no hemos
@@ -1115,7 +1116,7 @@
 DT</t>
   </si>
   <si>
-    <t>Quería proporcionar una actualización sobre nuestro progreso con AEC. Bryce Baxter y su
+    <t xml:space="preserve">Quería proporcionar una actualización sobre nuestro progreso con AEC. Bryce Baxter y su
 los miembros del equipo han estado en contacto con Mike Bennett y Bill Hogue para
 Comprender sus necesidades. Hemos proporcionado la información inicial que
 solicitado (es decir, un mes de datos), y están esperando su aprobación antes
@@ -1126,7 +1127,7 @@
 Susan</t>
   </si>
   <si>
-    <t>Robar,
+    <t xml:space="preserve">Robar,
 Gracias por traer esto a mi atención. Me reuní con los miembros de mi equipo esta
 mañana y hemos hecho una llamada a AEC. Te informaré del resultado
 de la situación tan pronto como se resuelva.
@@ -1138,7 +1139,7 @@
 713-853-3960</t>
   </si>
   <si>
-    <t>Susan, entiendo que Isabel Recindes, Drew Hill, Gerno Mendosa, Michelle
+    <t xml:space="preserve">Susan, entiendo que Isabel Recindes, Drew Hill, Gerno Mendosa, Michelle
 Stevens y Sherry Thomas pueden informar directamente a usted. Uno de los de Enron Canadá
 Los clientes clave (AEC) han intentado durante los últimos seis meses trabajar con
 arriba al obtener un desglose detallado con respecto a una transacción en curso
@@ -1152,7 +1153,7 @@
 Enron Canadá</t>
   </si>
   <si>
-    <t>Hola a todos,
+    <t xml:space="preserve">Hola a todos,
 Solo un recordatorio amistoso para reenviarme los nombres de aquellos a quienes les gustaría colocar
 los equipos de acción de ETC si aún no lo han hecho. Además, recuerda
 para especificar si está colocando a alguien en el equipo global o en el corporativo
@@ -1163,7 +1164,7 @@
 x3-3833</t>
   </si>
   <si>
-    <t>Mi equipo necesitará el fin de semana para organizar todo esto. Tendremos
+    <t xml:space="preserve">Mi equipo necesitará el fin de semana para organizar todo esto. Tendremos
 ellos lunes al final del día.
 Kim Melodick</t>
   </si>
@@ -1181,7 +1182,7 @@
 </t>
   </si>
   <si>
-    <t>02 de febrero de 2001
+    <t xml:space="preserve">02 de febrero de 2001
 LAS FORMAS DE EVALUACIÓN DEL DESEMPEÑO DE FIN DE AÑO 2000 SON DEBIDAS EN RECURSOS HUMANOS POR EL
 Por encima de la fecha. PARA EEL, EL PLAZO ES EL 31 DE ENERO DE 2001.
 Si aún no lo ha hecho, comience el proceso de retroalimentación
@@ -1221,7 +1222,7 @@
     WILSON, SHONA A</t>
   </si>
   <si>
-    <t>Hemos recibido varias consultas sobre el enlace de correo electrónico incrustado en el
+    <t xml:space="preserve">Hemos recibido varias consultas sobre el enlace de correo electrónico incrustado en el
 Comunicación distribuida el 27 de diciembre de 2000 por Steve Kean y Cindy Olson
 en referencia al proceso de la RPC. Si ha tenido problemas cuando
 haciendo clic en este enlace, copie y pegue el enlace en un mensaje de correo electrónico. Nosotros
@@ -1230,12 +1231,12 @@
 La dirección de correo electrónico para enviar sus ideas y sugerencias es perfmgmt@enron.com</t>
   </si>
   <si>
-    <t>Gracias sally Según la respuesta de Rick, puedo organizar la adición de nombres adicionales
+    <t xml:space="preserve">Gracias sally Según la respuesta de Rick, puedo organizar la adición de nombres adicionales
 para que pueda proporcionar comentarios. También le dejaré a Rick un correo de voz ...
 Sí</t>
   </si>
   <si>
-    <t>He completado formularios de comentarios internos a través del sistema PEP para Brent
+    <t xml:space="preserve">He completado formularios de comentarios internos a través del sistema PEP para Brent
 Price, Bob Hall y Peggy Hedstrom. Esos parecían ser los únicos nombres que
 incluiste para lo que querías mi opinión. De alguna manera, por la voz de Andrea
 mensaje de correo la semana pasada, había anticipado responder a más solicitudes - I
@@ -1247,13 +1248,13 @@
 como una solicitud cumplió con sus expectativas en términos de mi respuesta)</t>
   </si>
   <si>
-    <t>De acuerdo a lo pedido...
+    <t xml:space="preserve">De acuerdo a lo pedido...
 ¡Por favor hazme saber si tienes preguntas!
 Gracias
 Sheri</t>
   </si>
   <si>
-    <t>Pido disculpas por la notificación tardía, pero a Sally se le acaba de notificar que
+    <t xml:space="preserve">Pido disculpas por la notificación tardía, pero a Sally se le acaba de notificar que
 reunión de PRC interfuncional con Rick Causey se ha establecido para este viernes,
 1 de diciembre. Ella necesitará una compilación de tus logros
 Jueves. Si tiene directores que le informan, solicite que ellos
@@ -1262,7 +1263,7 @@
 Patti x39106</t>
   </si>
   <si>
-    <t>Hoy concluimos nuestra investigación sobre la renuncia de Jenny Lu.
+    <t xml:space="preserve">Hoy concluimos nuestra investigación sobre la renuncia de Jenny Lu.
 Hablamos con un total de cinco empleados. Dos fueron sugeridos por Jenny Lu
 (Vanessa Schultz y Wally Kinden) y tres sugeridos por Joel Henenberg
 (Mary Gosnell, Bill Hare y Connie Sutton). La investigación no
@@ -1275,7 +1276,7 @@
 Frank deJesus</t>
   </si>
   <si>
-    <t>Salida,
+    <t xml:space="preserve">Salida,
 Estos son los comentarios de los informes directos de Sheri Thomas. Esta bien escrito
 y constructivo Le dije a Dale que te lo enviaría y que estaba
 Seguro que agradecería los comentarios.
@@ -1290,7 +1291,7 @@
 memo abajo Gracias por su respuesta.</t>
   </si>
   <si>
-    <t>Creo que todos ustedes conocieron a Frank (cuyo apellido no recuerdo),
+    <t xml:space="preserve">Creo que todos ustedes conocieron a Frank (cuyo apellido no recuerdo),
 el generalista de recursos humanos que actualmente trabaja con Héctor para atender las necesidades de recursos humanos
 para Operaciones Energéticas en ENA. Frank está trabajando por contrato en este
 tiempo, y Sheila Walton está buscando comentarios sobre su desempeño hasta la fecha en
@@ -1303,7 +1304,7 @@
 tiempo de hacer esto.</t>
   </si>
   <si>
-    <t>Contratando administradores,
+    <t xml:space="preserve">Contratando administradores,
 Aquí hay algunos consejos que mejorarán inmediatamente el tiempo que lleva hacer una
 ofrezca a sus candidatos.
 Todos los solicitantes deben completar y firmar una Solicitud y un Crédito Justo
@@ -1325,7 +1326,7 @@
 Equipo de Recursos Humanos de ENA Energy Ops</t>
   </si>
   <si>
-    <t>Héctor, esto es para verificar nuestra conversación sobre el aumento anual
+    <t xml:space="preserve">Héctor, esto es para verificar nuestra conversación sobre el aumento anual
 salario base para Jesse Villarreal de $ 50,160 a $ 56,000.
   Si es posible, procese el aumento para que entre en vigencia el 1 de octubre.
 Jesse es especialista en el centro de costos 105603 en la programación de Logistics East
@@ -1334,13 +1335,13 @@
 Avíseme si necesita información adicional, gracias - Bob Superty</t>
   </si>
   <si>
-    <t>Por favor, eche un vistazo a esta carta. Estamos cómodos con eso, pero necesitas
+    <t xml:space="preserve">Por favor, eche un vistazo a esta carta. Estamos cómodos con eso, pero necesitas
 estar bien antes de que se envíe. Siéntase libre de proponer cualquier cambio. De otra manera
 Puedes dejarlo volar.
 Brian</t>
   </si>
   <si>
-    <t>Estimadas operaciones de energía:
+    <t xml:space="preserve">Estimadas operaciones de energía:
 Como he reflexionado sobre los logros de este grupo, quería
 expreso mi agradecimiento por todo el trabajo duro y la dedicación que tiene
 demostrado Hemos hecho un gran trabajo y quiero reconocerte por eso.
@@ -1371,7 +1372,7 @@
 tú.</t>
   </si>
   <si>
-    <t>Comuníquese conmigo para determinar el ajuste salarial que desea dar a
+    <t xml:space="preserve">Comuníquese conmigo para determinar el ajuste salarial que desea dar a
 su empleado recién ascendido. Si el empleado ha sido promovido fuera de
 su departamento pero aún está dentro de ENA, por favor envíe este correo electrónico a su
 Jefe de departamento actual.
@@ -1382,7 +1383,7 @@
 Gracias por su ayuda en este asunto</t>
   </si>
   <si>
-    <t>A LA CONTRATACIÓN DE GERENTES Y ASISTENTES, (Reenvíe a cualquiera
+    <t xml:space="preserve">A LA CONTRATACIÓN DE GERENTES Y ASISTENTES, (Reenvíe a cualquiera
 incluido.)
 ¡Nuevo! Formulario de solicitud de personal:
 Con la implementación de SAP, este formulario es ahora el factor clave crítico para
@@ -1415,7 +1416,7 @@
 ENA Commerc</t>
   </si>
   <si>
-    <t>Esta nota responde a su reciente solicitud de actualización de estado en Sandra
+    <t xml:space="preserve">Esta nota responde a su reciente solicitud de actualización de estado en Sandra
 Dial y su deseo de seguir un programa de MBA ejecutivo en la Universidad de Rice.
 En seguimiento a la discusión mantenida con Sandra Dial, Sally Beck y yo
 el 21 de abril de 2000, Sally le indicó a Sandra que mientras ella fuertemente
@@ -1429,14 +1430,14 @@
 Intención de renuncia. Como resultado, el proceso se ha detenido.</t>
   </si>
   <si>
-    <t>Todd
+    <t xml:space="preserve">Todd
 Vamos a elaborar un plan mañana para los gerentes de Jeff Gossett antes del
 completar su encuesta. Si su horario no lo permite, por favor
 recomendar a alguien en comp. quién puede ayudar o proporcionar orientación para
 alternativas. Gracias por tu ayuda.</t>
   </si>
   <si>
-    <t>Héctor: Los empleados clave que Jeff ha identificado son especialistas senior,
+    <t xml:space="preserve">Héctor: Los empleados clave que Jeff ha identificado son especialistas senior,
 con la excepción de Will Kelly. Si recuerdas, estos son el riesgo
 empleados que me preocupaban cuando Steve Jackson presentó su carta
 de resignación. Steve asumirá un papel similar con un competidor, y
@@ -1447,7 +1448,7 @@
 acerca de cómo podemos comenzar esto. Gracias</t>
   </si>
   <si>
-    <t>Jeff
+    <t xml:space="preserve">Jeff
 Hablé con Todd Burke sobre una estrategia de retención para los gerentes que
 hablado sobre. Me dijo que haría una recomendación después de que él
 completa las prácticas de pago a mediados de noviembre a fin de
@@ -1457,7 +1458,7 @@
 que los gerentes están haciendo ofertas, entonces háganos saber.</t>
   </si>
   <si>
-    <t>Hay algunas personas clave que creo que son esenciales para lograr nuestros objetivos.
+    <t xml:space="preserve">Hay algunas personas clave que creo que son esenciales para lograr nuestros objetivos.
 en gestión de riesgos de gas. Son :
 Will Kelly
 Kam Keizer
@@ -1472,7 +1473,7 @@
 Gracias,</t>
   </si>
   <si>
-    <t>Este es el estado actual de las evaluaciones de desempeño pendientes.
+    <t xml:space="preserve">Este es el estado actual de las evaluaciones de desempeño pendientes.
 Michelle Cash está revisando lo siguiente:
 Chris Mendoza
 Ron Gaskey
@@ -1492,7 +1493,7 @@
 primero.</t>
   </si>
   <si>
-    <t>¡Buenas noticias!
+    <t xml:space="preserve">¡Buenas noticias!
 Ha sido seleccionado para recibir U S $ 1 , 2 8 0 , 0 0 0 . 0 0. Para recibir la subvención envíenos su número de referencia por correo electrónico.
 revdiego@nationalaward.org
 Número de referencia:   DP108-02777 
@@ -1500,7 +1501,7 @@
 Rev.Diego Organización.</t>
   </si>
   <si>
-    <t>Responda una pequeña encuesta y gane $5
+    <t xml:space="preserve">Responda una pequeña encuesta y gane $5
 Nos gustaría conocer su opinión. Como agradecimiento por responder a esta encuesta, recibirá una tarjeta de regalo con $5 de Visa. Tome en cuenta que usted debe ser elegible y completar toda la encuesta para recibir la tarjeta de regalo.
 Este estudio confidencial se está realizando en la plataforma de encuestas de Qualtrics en representación de un cliente, un líder de la industria de la tecnología, para entender mejor cuánto significan para usted sus servicios. Responder esta encuesta le tomará aproximadamente de 20 a 25 minutos.
 Haga clic abajo para comenzar o copie y pegue el enlace en su navegador de internet.
@@ -1508,11 +1509,11 @@
 Muchas gracias. Le agradecemos por su tiempo.</t>
   </si>
   <si>
-    <t>Estimado(a): ocejo
+    <t xml:space="preserve">Estimado(a): ocejo
 Le informamos que nuestros sistemas han detectado un inconveniente con su dispositivo TOKEN, por lo que se requiere sincronizar ahora. Este procedimiento solo será solicitado por única vez, ya que garantiza la protección de sus datos de por vida y no será necesario solicitarla nuevamente.</t>
   </si>
   <si>
-    <t>Saludos a ti mi querido amigo.
+    <t xml:space="preserve">Saludos a ti mi querido amigo.
 Mi nombre es la Sra. Mariam Konta, una viuda que padece una enfermedad
 de cáncer. Le escribo este correo con lágrimas serias en los ojos y
 una gran pena en mi corazón. Decidí contactarlo debido a la urgencia
@@ -1522,18 +1523,72 @@
 Por favor responda para más detalles
 Mrs Mariam Konta</t>
   </si>
+  <si>
+    <t xml:space="preserve">Para BBVA la máxima prioridad son nuestros empleados, nuestros clientes y nuestros usuarios.  La experiencia internacional ha demostrado que la medida más efectiva para detener el contagio es evitar la concentración de personas. Por ello, hemos desarrollado un plan para disminuir el riesgo de propagación del COVID-19 sin afectaciones al servicio.  Solo el personal cuya función es indispensable para dar continuidad a la operación asistirá a los edificios corporativos, con todas las medidas de prevención necesarias.  Mantendremos en operación el mayor número posible de sucursales, aunque con el mínimo de personal para garantizar los protocolos de seguridad y de servicio en las operaciones de los clientes.  Ponemos a disposición de nuestros clientes y usuarios los servicios de banca digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tu token móvil fue ACTIVADO, comienza a disfrutar de los beneficios de bbva.mx, te compartimos los detalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La activación del servicio de app BBVA fue exitosa, te compartimos los detalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buenos días profesor De Luna Caballero,     Mi nombre es Eduardo Macedo y junto con mis compañeros César Gasca y Roger Morales desarrollamos el Trabajo Terminal 2 del TT 2019-A013  “Extensión de navegador web para detectar ataques de phishing en correos en español” del cual usted quedó asignado como Director de Seguimiento en el actual semestre.     Quisiéramos preguntarle ¿en qué horario  sería posible concertar una junta para poder platicar formalmente de cómo le gustaría que trabajásemos?     Aprovechando para comentarle que los 3 integrantes trabajamos y tenemos disponible solamente el horario vespertino, le comentamos para nosotros poder acomodarnos a los horarios que nos diga.     Gracias de antemano por su atención y de ser necesario  lo podemos pasar a ver para platicar también.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hola , Paco. Ya agregué a los alumnos pero hubo algunas incidencias con respecto a los profes ya que no están agregados o superan el máximo de alumnos. Te mando una lista con las incidencias que te menciono.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hola  César,     Espero te encuentres muy bien, el motivo de mi correo es para darle seguimiento a tu proceso que iniciaste con nocotros el día de tu visita a lnuestras oficinas. Antes que nada te agradezco tu tiempo y el interés que demostraste, valoramos mucho que hayas participado en nuestra actividad y esperamos que haya sido lo que esperabas, de igualmanera cualquier retroalimentación o comentario nos lo puedes hacer llegar por este medio.       Al iniciar el proceso te postulaste a la vacante de desarrollo te comento, actualmente no contamos con esta vacante, sin embargo estamos por iniciar un nuevo año con un plan nuevo de reclutamiento y se puede abrir en un futuro, si tu gustas puedes estar en nuestra base para próximas ocasiones. Como sabemos que puede ser la primera vez que inicias un proceso te dare una pequeña retroalimentación para futuras ocasiones: como recomendación sería evitar un poco los nervios ya que tienes un buen perfil y en el examen aplicado saliste muy bien, por esta ocasión la principal razón por la que no podemos continuar con el proceso es por la falta de vacantes pero en general tienes un buen perfil para crecer y poder tener mayores conocimientos, te recomiendo poder aprender las tecnologías del momento para complementar tu perfil.     Una vez más agradezco tu participación, recuerda que puedes continuar tu proceso en otra ocasión y cualquier duda que tengas lo puedes consultar conmigo.     Quedo al pendiente de tus comentarios.     Saludos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hola Chicos: les comento que me prestan el aula 2213 a partir de las 12:00  hasta las 15:00 hrspor si alguno quiere entregar. su proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buen día chicos: Les aviso que durante esta semana no asistiré a clases por situaciones familiares. Inviertan esta semana en sus proyectos. Nos vemos el miércoles 20 de noviembre en nuestro horario normal  de clases.  Agradezco su apoyo y comprensión.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saludos, por medio del presente correo les estoy haciendo llegar el archivo en corel, del circuito con el que aprenderemos a fabricar circuitos impresos.   Hasta pronto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saludos, aquí les estoy adjuntando el formato de la siguiente práctica a realizarse el próximo día lunes.   Hasta pronto.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoy se aplica el examen teorico saludos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saludos, aquí les estoy adjuntando 2 materiales para que puedan realizar la practica del próximo lunes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1545,7 +1600,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -1553,1051 +1608,919 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A103" activeCellId="0" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="255.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="240" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B18" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B23" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B25" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B27" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B28" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B29" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B30" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B31" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B32" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B33" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B34" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B35" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B36" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B37" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="342" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B38" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B40" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B41" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B42" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B43" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B44" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B45" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B46" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B47" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B48" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B49" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B50" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B51" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B52" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B54" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B56" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B56" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B57" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B59" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B59" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B62" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B62" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B64" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B64" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B65" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="B65" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="285" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B66" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B66" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B67" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B67" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B68" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B69" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+      <c r="B69" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="315" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B70" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B70" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B71" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="B71" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B72" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B72" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B73" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B73" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B74" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B74" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B75" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="B75" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B76" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B76" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B77" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B77" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B78" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B78" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B79" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="B79" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="375" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B80" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B80" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B81" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B81" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B82" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B82" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B83" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B83" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B84" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B84" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B85" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B85" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B86" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B86" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B87" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B87" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B88" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B88" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B89" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B89" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B90" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B90" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B91" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B91" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B92" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B92" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B93" t="s">
-        <v>3</v>
+      <c r="B93" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="A95" r:id="rId1" display="bbva.mx"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>